<commit_message>
new version of multivendor added
</commit_message>
<xml_diff>
--- a/opencart_codebase/admin/view/image/admin_purpletree_bulk_product_upload.xlsx
+++ b/opencart_codebase/admin/view/image/admin_purpletree_bulk_product_upload.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365"/>
+    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,12 @@
     <sheet name="ProductOption" sheetId="12" r:id="rId12"/>
     <sheet name="ProductOptionValue" sheetId="13" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="89">
   <si>
     <t>product_id</t>
   </si>
@@ -74,9 +74,6 @@
   </si>
   <si>
     <t>demo 678</t>
-  </si>
-  <si>
-    <t>add_product</t>
   </si>
   <si>
     <t>model</t>
@@ -301,8 +298,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -468,7 +465,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -503,7 +499,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -679,17 +674,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="8" style="2" customWidth="1"/>
@@ -701,7 +696,7 @@
     <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="24.95" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -724,10 +719,10 @@
         <v>6</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>93</v>
       </c>
@@ -744,7 +739,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>97</v>
       </c>
@@ -767,7 +762,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>98</v>
       </c>
@@ -797,7 +792,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -807,33 +802,33 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="24.95" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>93</v>
       </c>
       <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" t="s">
         <v>78</v>
-      </c>
-      <c r="C2" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -843,7 +838,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -853,38 +848,38 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="24.95" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>93</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>93</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -894,7 +889,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -904,7 +899,7 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="8" style="2" customWidth="1"/>
@@ -913,7 +908,7 @@
     <col min="5" max="5" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="24.95" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -921,13 +916,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -937,7 +932,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -947,7 +942,7 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
@@ -961,39 +956,39 @@
     <col min="11" max="11" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="24.95" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1003,54 +998,53 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AE4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="7" width="7" customWidth="1"/>
-    <col min="8" max="8" width="8" customWidth="1"/>
-    <col min="9" max="9" width="7" customWidth="1"/>
-    <col min="10" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="16" customWidth="1"/>
-    <col min="13" max="13" width="9" customWidth="1"/>
-    <col min="14" max="14" width="16" customWidth="1"/>
-    <col min="15" max="15" width="12" customWidth="1"/>
-    <col min="16" max="16" width="9" customWidth="1"/>
-    <col min="17" max="17" width="20" customWidth="1"/>
-    <col min="18" max="18" width="15" customWidth="1"/>
-    <col min="19" max="19" width="10" customWidth="1"/>
-    <col min="20" max="20" width="13" customWidth="1"/>
-    <col min="21" max="21" width="18" style="2" customWidth="1"/>
-    <col min="22" max="22" width="10" customWidth="1"/>
-    <col min="23" max="23" width="16" customWidth="1"/>
-    <col min="24" max="24" width="10" customWidth="1"/>
-    <col min="25" max="25" width="9" customWidth="1"/>
-    <col min="26" max="26" width="10" customWidth="1"/>
-    <col min="27" max="27" width="16" customWidth="1"/>
-    <col min="28" max="28" width="12" customWidth="1"/>
-    <col min="29" max="29" width="11" customWidth="1"/>
-    <col min="30" max="30" width="14" customWidth="1"/>
-    <col min="31" max="31" width="10" customWidth="1"/>
-    <col min="32" max="32" width="9" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="3" max="6" width="7" customWidth="1"/>
+    <col min="7" max="7" width="8" customWidth="1"/>
+    <col min="8" max="8" width="7" customWidth="1"/>
+    <col min="9" max="10" width="12" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
+    <col min="12" max="12" width="9" customWidth="1"/>
+    <col min="13" max="13" width="16" customWidth="1"/>
+    <col min="14" max="14" width="12" customWidth="1"/>
+    <col min="15" max="15" width="9" customWidth="1"/>
+    <col min="16" max="16" width="20" customWidth="1"/>
+    <col min="17" max="17" width="15" customWidth="1"/>
+    <col min="18" max="18" width="10" customWidth="1"/>
+    <col min="19" max="19" width="13" customWidth="1"/>
+    <col min="20" max="20" width="18" style="2" customWidth="1"/>
+    <col min="21" max="21" width="10" customWidth="1"/>
+    <col min="22" max="22" width="16" customWidth="1"/>
+    <col min="23" max="23" width="10" customWidth="1"/>
+    <col min="24" max="24" width="9" customWidth="1"/>
+    <col min="25" max="25" width="10" customWidth="1"/>
+    <col min="26" max="26" width="16" customWidth="1"/>
+    <col min="27" max="27" width="12" customWidth="1"/>
+    <col min="28" max="28" width="11" customWidth="1"/>
+    <col min="29" max="29" width="14" customWidth="1"/>
+    <col min="30" max="30" width="10" customWidth="1"/>
+    <col min="31" max="31" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" ht="24.95" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>17</v>
@@ -1103,10 +1097,10 @@
       <c r="S1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="1" t="s">
         <v>35</v>
       </c>
       <c r="V1" s="1" t="s">
@@ -1139,170 +1133,167 @@
       <c r="AE1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AF1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:31">
+      <c r="A2">
+        <v>93</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2">
+        <v>10</v>
+      </c>
+      <c r="K2" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B2">
-        <v>93</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2">
-        <v>10</v>
       </c>
       <c r="L2" t="s">
         <v>47</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>48</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2">
+        <v>250</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>500</v>
+      </c>
+      <c r="T2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="P2">
-        <v>250</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>500</v>
-      </c>
-      <c r="U2" s="2" t="s">
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2" t="s">
         <v>50</v>
       </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="W2" t="s">
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2" t="s">
         <v>51</v>
       </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-      <c r="Z2">
-        <v>0</v>
-      </c>
       <c r="AA2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="AB2">
+        <v>1</v>
       </c>
       <c r="AC2">
         <v>1</v>
       </c>
-      <c r="AD2">
-        <v>1</v>
-      </c>
-      <c r="AE2" t="s">
+      <c r="AD2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31">
+      <c r="A3">
+        <v>97</v>
+      </c>
+      <c r="B3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>97</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="N3" t="s">
         <v>54</v>
       </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="O3" t="s">
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="T3" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="U3" s="2" t="s">
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3" t="s">
         <v>56</v>
       </c>
-      <c r="V3">
-        <v>0</v>
-      </c>
-      <c r="X3">
-        <v>0</v>
-      </c>
-      <c r="Y3">
-        <v>0</v>
-      </c>
-      <c r="Z3">
-        <v>0</v>
-      </c>
-      <c r="AB3" t="s">
+    </row>
+    <row r="4" spans="1:31">
+      <c r="A4">
+        <v>98</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="N4" t="s">
+        <v>54</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="T4" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AC3">
-        <v>0</v>
-      </c>
-      <c r="AD3">
-        <v>0</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>98</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="AA4" t="s">
         <v>54</v>
       </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="O4" t="s">
-        <v>55</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="U4" s="2" t="s">
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4" t="s">
         <v>56</v>
-      </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
-      <c r="Y4">
-        <v>0</v>
-      </c>
-      <c r="Z4">
-        <v>0</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC4">
-        <v>0</v>
-      </c>
-      <c r="AD4">
-        <v>0</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1312,7 +1303,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1322,7 +1313,7 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="3" width="12" style="2" customWidth="1"/>
@@ -1331,51 +1322,51 @@
     <col min="6" max="6" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="24.95" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>93</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" t="s">
         <v>63</v>
       </c>
-      <c r="F2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>97</v>
       </c>
       <c r="F3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>98</v>
       </c>
       <c r="F4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1385,7 +1376,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1395,22 +1386,22 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="8" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="24.95" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1420,7 +1411,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1430,22 +1421,22 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="24.95" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1455,7 +1446,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1465,7 +1456,7 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
@@ -1476,30 +1467,30 @@
     <col min="8" max="8" width="12" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="24.95" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1509,7 +1500,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1519,7 +1510,7 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
@@ -1530,27 +1521,27 @@
     <col min="7" max="7" width="12" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="24.95" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1560,7 +1551,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1570,7 +1561,7 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
@@ -1578,21 +1569,21 @@
     <col min="4" max="4" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="24.95" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>2663</v>
       </c>
@@ -1600,13 +1591,13 @@
         <v>93</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2662</v>
       </c>
@@ -1614,7 +1605,7 @@
         <v>93</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1627,7 +1618,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1637,30 +1628,30 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="24.95" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>93</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2">
         <v>300</v>

</xml_diff>